<commit_message>
Upgrade: Recursive lag/rolling/cyclical forecasting in app and model
</commit_message>
<xml_diff>
--- a/rf_test_vs_prediction_results.xlsx
+++ b/rf_test_vs_prediction_results.xlsx
@@ -462,7 +462,7 @@
         <v>4.857571407053999</v>
       </c>
       <c r="C2" t="n">
-        <v>5.387076929282244</v>
+        <v>5.357014073982379</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         <v>4.668443393714001</v>
       </c>
       <c r="C3" t="n">
-        <v>5.400197302053832</v>
+        <v>5.41150300847178</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +484,7 @@
         <v>4.80551908429409</v>
       </c>
       <c r="C4" t="n">
-        <v>5.387623819316834</v>
+        <v>5.38941312044156</v>
       </c>
     </row>
     <row r="5">
@@ -495,7 +495,7 @@
         <v>4.998026813941</v>
       </c>
       <c r="C5" t="n">
-        <v>5.325835421096413</v>
+        <v>5.41322479766224</v>
       </c>
     </row>
     <row r="6">
@@ -506,7 +506,7 @@
         <v>5.023363338918999</v>
       </c>
       <c r="C6" t="n">
-        <v>5.368900836512113</v>
+        <v>5.448597060608876</v>
       </c>
     </row>
     <row r="7">
@@ -517,7 +517,7 @@
         <v>4.822616096114</v>
       </c>
       <c r="C7" t="n">
-        <v>5.251247144839189</v>
+        <v>5.442691260659217</v>
       </c>
     </row>
     <row r="8">
@@ -528,7 +528,7 @@
         <v>4.429607166733</v>
       </c>
       <c r="C8" t="n">
-        <v>5.247900515506589</v>
+        <v>5.389662639061666</v>
       </c>
     </row>
     <row r="9">
@@ -539,7 +539,7 @@
         <v>5.438515029533001</v>
       </c>
       <c r="C9" t="n">
-        <v>5.352532766237604</v>
+        <v>5.33495519513759</v>
       </c>
     </row>
     <row r="10">
@@ -550,7 +550,7 @@
         <v>5.185118522125</v>
       </c>
       <c r="C10" t="n">
-        <v>5.282123806886058</v>
+        <v>5.206862627700581</v>
       </c>
     </row>
     <row r="11">
@@ -561,7 +561,7 @@
         <v>5.692019099825</v>
       </c>
       <c r="C11" t="n">
-        <v>5.478138081273582</v>
+        <v>5.487225718056448</v>
       </c>
     </row>
     <row r="12">
@@ -572,7 +572,7 @@
         <v>5.223532946875</v>
       </c>
       <c r="C12" t="n">
-        <v>5.361522091281227</v>
+        <v>5.365576215073335</v>
       </c>
     </row>
     <row r="13">
@@ -583,7 +583,7 @@
         <v>5.418027537625001</v>
       </c>
       <c r="C13" t="n">
-        <v>5.395901476668318</v>
+        <v>5.390407686401995</v>
       </c>
     </row>
     <row r="14">
@@ -594,7 +594,7 @@
         <v>5.840909350502</v>
       </c>
       <c r="C14" t="n">
-        <v>5.438268948230167</v>
+        <v>5.355795346413182</v>
       </c>
     </row>
     <row r="15">
@@ -605,7 +605,7 @@
         <v>5.560000497824999</v>
       </c>
       <c r="C15" t="n">
-        <v>5.448695486976484</v>
+        <v>5.392858265446741</v>
       </c>
     </row>
     <row r="16">
@@ -616,7 +616,7 @@
         <v>5.76415121375</v>
       </c>
       <c r="C16" t="n">
-        <v>5.444048782275079</v>
+        <v>5.389221991429598</v>
       </c>
     </row>
     <row r="17">
@@ -627,7 +627,7 @@
         <v>5.407662430525001</v>
       </c>
       <c r="C17" t="n">
-        <v>5.336219128130523</v>
+        <v>5.37248258621656</v>
       </c>
     </row>
     <row r="18">
@@ -638,7 +638,7 @@
         <v>5.635396825932</v>
       </c>
       <c r="C18" t="n">
-        <v>5.342992789302098</v>
+        <v>5.424286086096097</v>
       </c>
     </row>
     <row r="19">
@@ -649,7 +649,7 @@
         <v>5.904906289082</v>
       </c>
       <c r="C19" t="n">
-        <v>5.202300799875214</v>
+        <v>5.35595697147806</v>
       </c>
     </row>
     <row r="20">
@@ -660,7 +660,7 @@
         <v>5.754983475486</v>
       </c>
       <c r="C20" t="n">
-        <v>5.168086080966206</v>
+        <v>5.199697252903536</v>
       </c>
     </row>
     <row r="21">
@@ -671,7 +671,7 @@
         <v>6.125426000894999</v>
       </c>
       <c r="C21" t="n">
-        <v>5.299607916720249</v>
+        <v>5.288476628738822</v>
       </c>
     </row>
     <row r="22">
@@ -682,7 +682,7 @@
         <v>5.406917101506</v>
       </c>
       <c r="C22" t="n">
-        <v>5.335939805030911</v>
+        <v>5.340979444556811</v>
       </c>
     </row>
     <row r="23">
@@ -693,7 +693,7 @@
         <v>6.574890841338999</v>
       </c>
       <c r="C23" t="n">
-        <v>5.452216286427069</v>
+        <v>5.468636852298284</v>
       </c>
     </row>
     <row r="24">
@@ -704,7 +704,7 @@
         <v>6.405723786886</v>
       </c>
       <c r="C24" t="n">
-        <v>5.313599142040866</v>
+        <v>5.345374103807838</v>
       </c>
     </row>
     <row r="25">
@@ -715,7 +715,7 @@
         <v>6.718604456511001</v>
       </c>
       <c r="C25" t="n">
-        <v>5.393447153929418</v>
+        <v>5.434093945178742</v>
       </c>
     </row>
     <row r="26">
@@ -726,7 +726,7 @@
         <v>6.05485169882</v>
       </c>
       <c r="C26" t="n">
-        <v>5.445048591486604</v>
+        <v>5.362032325931564</v>
       </c>
     </row>
     <row r="27">
@@ -737,7 +737,7 @@
         <v>5.72217794552</v>
       </c>
       <c r="C27" t="n">
-        <v>5.423779320221655</v>
+        <v>5.370758244473357</v>
       </c>
     </row>
     <row r="28">
@@ -748,7 +748,7 @@
         <v>6.699475908175</v>
       </c>
       <c r="C28" t="n">
-        <v>5.410396997102859</v>
+        <v>5.341080634174729</v>
       </c>
     </row>
     <row r="29">
@@ -759,7 +759,7 @@
         <v>5.647809795596</v>
       </c>
       <c r="C29" t="n">
-        <v>5.361264895745361</v>
+        <v>5.437915057973232</v>
       </c>
     </row>
     <row r="30">
@@ -770,7 +770,7 @@
         <v>5.854452414233</v>
       </c>
       <c r="C30" t="n">
-        <v>5.376502428808776</v>
+        <v>5.442685068230362</v>
       </c>
     </row>
     <row r="31">
@@ -781,7 +781,7 @@
         <v>5.460436904519</v>
       </c>
       <c r="C31" t="n">
-        <v>5.203201836917231</v>
+        <v>5.433941970145027</v>
       </c>
     </row>
     <row r="32">
@@ -792,7 +792,7 @@
         <v>5.755830683622917</v>
       </c>
       <c r="C32" t="n">
-        <v>5.20793591288171</v>
+        <v>5.369472881507372</v>
       </c>
     </row>
     <row r="33">
@@ -803,7 +803,7 @@
         <v>5.991571160172917</v>
       </c>
       <c r="C33" t="n">
-        <v>5.409128490409967</v>
+        <v>5.441959514437273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial commit for Natural Gas Price Forecasting app
</commit_message>
<xml_diff>
--- a/rf_test_vs_prediction_results.xlsx
+++ b/rf_test_vs_prediction_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,354 +456,409 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44774</v>
+        <v>44621</v>
       </c>
       <c r="B2" t="n">
-        <v>4.857571407053999</v>
+        <v>4.979304347826087</v>
       </c>
       <c r="C2" t="n">
-        <v>5.357014073982379</v>
+        <v>3.527235960897797</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44805</v>
+        <v>44652</v>
       </c>
       <c r="B3" t="n">
-        <v>4.668443393714001</v>
+        <v>6.704599999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>5.41150300847178</v>
+        <v>3.333792138622242</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44835</v>
+        <v>44682</v>
       </c>
       <c r="B4" t="n">
-        <v>4.80551908429409</v>
+        <v>8.163476190476191</v>
       </c>
       <c r="C4" t="n">
-        <v>5.38941312044156</v>
+        <v>3.869712129587803</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44866</v>
+        <v>44713</v>
       </c>
       <c r="B5" t="n">
-        <v>4.998026813941</v>
+        <v>7.597904761904761</v>
       </c>
       <c r="C5" t="n">
-        <v>5.41322479766224</v>
+        <v>3.837306424712959</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44896</v>
+        <v>44743</v>
       </c>
       <c r="B6" t="n">
-        <v>5.023363338918999</v>
+        <v>7.186949999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>5.448597060608876</v>
+        <v>4.002185601025777</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44927</v>
+        <v>44774</v>
       </c>
       <c r="B7" t="n">
-        <v>4.822616096114</v>
+        <v>8.779478260869567</v>
       </c>
       <c r="C7" t="n">
-        <v>5.442691260659217</v>
+        <v>4.013261431441737</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44958</v>
+        <v>44805</v>
       </c>
       <c r="B8" t="n">
-        <v>4.429607166733</v>
+        <v>7.757523809523809</v>
       </c>
       <c r="C8" t="n">
-        <v>5.389662639061666</v>
+        <v>3.226247721155653</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44986</v>
+        <v>44835</v>
       </c>
       <c r="B9" t="n">
-        <v>5.438515029533001</v>
+        <v>6.084904761904762</v>
       </c>
       <c r="C9" t="n">
-        <v>5.33495519513759</v>
+        <v>4.331143578016185</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45017</v>
+        <v>44866</v>
       </c>
       <c r="B10" t="n">
-        <v>5.185118522125</v>
+        <v>6.429761904761905</v>
       </c>
       <c r="C10" t="n">
-        <v>5.206862627700581</v>
+        <v>4.088435594108788</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45047</v>
+        <v>44896</v>
       </c>
       <c r="B11" t="n">
-        <v>5.692019099825</v>
+        <v>5.768047619047617</v>
       </c>
       <c r="C11" t="n">
-        <v>5.487225718056448</v>
+        <v>3.862876669066445</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45078</v>
+        <v>44927</v>
       </c>
       <c r="B12" t="n">
-        <v>5.223532946875</v>
+        <v>3.4228</v>
       </c>
       <c r="C12" t="n">
-        <v>5.365576215073335</v>
+        <v>3.831679320816868</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45108</v>
+        <v>44958</v>
       </c>
       <c r="B13" t="n">
-        <v>5.418027537625001</v>
+        <v>2.437473684210526</v>
       </c>
       <c r="C13" t="n">
-        <v>5.390407686401995</v>
+        <v>3.100549805568762</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45139</v>
+        <v>44986</v>
       </c>
       <c r="B14" t="n">
-        <v>5.840909350502</v>
+        <v>2.407782608695652</v>
       </c>
       <c r="C14" t="n">
-        <v>5.355795346413182</v>
+        <v>3.756926759975536</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45170</v>
+        <v>45017</v>
       </c>
       <c r="B15" t="n">
-        <v>5.560000497824999</v>
+        <v>2.197263157894737</v>
       </c>
       <c r="C15" t="n">
-        <v>5.392858265446741</v>
+        <v>3.68522301811594</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45200</v>
+        <v>45047</v>
       </c>
       <c r="B16" t="n">
-        <v>5.76415121375</v>
+        <v>2.299318181818181</v>
       </c>
       <c r="C16" t="n">
-        <v>5.389221991429598</v>
+        <v>3.878733911114246</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45231</v>
+        <v>45078</v>
       </c>
       <c r="B17" t="n">
-        <v>5.407662430525001</v>
+        <v>2.474619047619047</v>
       </c>
       <c r="C17" t="n">
-        <v>5.37248258621656</v>
+        <v>3.93739850879917</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45261</v>
+        <v>45108</v>
       </c>
       <c r="B18" t="n">
-        <v>5.635396825932</v>
+        <v>2.63655</v>
       </c>
       <c r="C18" t="n">
-        <v>5.424286086096097</v>
+        <v>3.987915421795595</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45292</v>
+        <v>45139</v>
       </c>
       <c r="B19" t="n">
-        <v>5.904906289082</v>
+        <v>2.645130434782609</v>
       </c>
       <c r="C19" t="n">
-        <v>5.35595697147806</v>
+        <v>4.12315972675513</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45323</v>
+        <v>45170</v>
       </c>
       <c r="B20" t="n">
-        <v>5.754983475486</v>
+        <v>2.69565</v>
       </c>
       <c r="C20" t="n">
-        <v>5.199697252903536</v>
+        <v>4.293742952757388</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45352</v>
+        <v>45200</v>
       </c>
       <c r="B21" t="n">
-        <v>6.125426000894999</v>
+        <v>3.149181818181818</v>
       </c>
       <c r="C21" t="n">
-        <v>5.288476628738822</v>
+        <v>4.467400830792398</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45383</v>
+        <v>45231</v>
       </c>
       <c r="B22" t="n">
-        <v>5.406917101506</v>
+        <v>3.055523809523809</v>
       </c>
       <c r="C22" t="n">
-        <v>5.340979444556811</v>
+        <v>4.366577304441936</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45413</v>
+        <v>45261</v>
       </c>
       <c r="B23" t="n">
-        <v>6.574890841338999</v>
+        <v>2.53885</v>
       </c>
       <c r="C23" t="n">
-        <v>5.468636852298284</v>
+        <v>4.013489311170718</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45444</v>
+        <v>45292</v>
       </c>
       <c r="B24" t="n">
-        <v>6.405723786886</v>
+        <v>2.715</v>
       </c>
       <c r="C24" t="n">
-        <v>5.345374103807838</v>
+        <v>3.871865006587618</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45474</v>
+        <v>45323</v>
       </c>
       <c r="B25" t="n">
-        <v>6.718604456511001</v>
+        <v>1.7955</v>
       </c>
       <c r="C25" t="n">
-        <v>5.434093945178742</v>
+        <v>3.824713038631661</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45505</v>
+        <v>45352</v>
       </c>
       <c r="B26" t="n">
-        <v>6.05485169882</v>
+        <v>1.7473</v>
       </c>
       <c r="C26" t="n">
-        <v>5.362032325931564</v>
+        <v>3.800614450969322</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45536</v>
+        <v>45383</v>
       </c>
       <c r="B27" t="n">
-        <v>5.72217794552</v>
+        <v>1.791227272727273</v>
       </c>
       <c r="C27" t="n">
-        <v>5.370758244473357</v>
+        <v>3.730415230190097</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45566</v>
+        <v>45413</v>
       </c>
       <c r="B28" t="n">
-        <v>6.699475908175</v>
+        <v>2.418</v>
       </c>
       <c r="C28" t="n">
-        <v>5.341080634174729</v>
+        <v>3.963432612460003</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45597</v>
+        <v>45444</v>
       </c>
       <c r="B29" t="n">
-        <v>5.647809795596</v>
+        <v>2.809578947368421</v>
       </c>
       <c r="C29" t="n">
-        <v>5.437915057973232</v>
+        <v>4.126224068275928</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45627</v>
+        <v>45474</v>
       </c>
       <c r="B30" t="n">
-        <v>5.854452414233</v>
+        <v>2.208681818181818</v>
       </c>
       <c r="C30" t="n">
-        <v>5.442685068230362</v>
+        <v>4.165283218379448</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45658</v>
+        <v>45505</v>
       </c>
       <c r="B31" t="n">
-        <v>5.460436904519</v>
+        <v>2.086782608695652</v>
       </c>
       <c r="C31" t="n">
-        <v>5.433941970145027</v>
+        <v>4.12398052964427</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45689</v>
+        <v>45536</v>
       </c>
       <c r="B32" t="n">
-        <v>5.755830683622917</v>
+        <v>2.409250000000001</v>
       </c>
       <c r="C32" t="n">
-        <v>5.369472881507372</v>
+        <v>4.544645989648032</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
+        <v>45566</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2.576956521739131</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4.481868937794092</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45597</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.982</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4.430318496141542</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>45627</v>
+      </c>
+      <c r="B35" t="n">
+        <v>3.406619047619048</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4.026412328816116</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>45658</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3.721380952380952</v>
+      </c>
+      <c r="C36" t="n">
+        <v>3.918379759034445</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45689</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3.740947368421053</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3.772891434406171</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
         <v>45717</v>
       </c>
-      <c r="B33" t="n">
-        <v>5.991571160172917</v>
-      </c>
-      <c r="C33" t="n">
-        <v>5.441959514437273</v>
+      <c r="B38" t="n">
+        <v>4.137476190476191</v>
+      </c>
+      <c r="C38" t="n">
+        <v>3.56765836274233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>